<commit_message>
updated the mina data set
</commit_message>
<xml_diff>
--- a/data/mina-data_06-07-22.xlsx
+++ b/data/mina-data_06-07-22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\projects\afib\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asshah4/projects/afib/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6756EC-DC90-4ADD-9F49-7F9FCEDB5291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBF0899-A00E-7E4E-9BB9-7862248992A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -82,11 +82,19 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color indexed="8"/>
+            <color rgb="FF000000"/>
             <rFont val="Helvetica Neue"/>
           </rPr>
-          <t>Mina Sous:
-3 attempts were tried</t>
+          <t xml:space="preserve">Mina Sous:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Helvetica Neue"/>
+          </rPr>
+          <t>3 attempts were tried</t>
         </r>
       </text>
     </comment>
@@ -449,7 +457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -469,6 +477,11 @@
     <font>
       <sz val="10"/>
       <color indexed="15"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -1801,19 +1814,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="7" width="16.36328125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.453125" style="1" customWidth="1"/>
-    <col min="10" max="39" width="16.36328125" style="1" customWidth="1"/>
-    <col min="40" max="16384" width="16.36328125" style="1"/>
+    <col min="1" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="17.5" style="1" customWidth="1"/>
+    <col min="10" max="39" width="16.33203125" style="1" customWidth="1"/>
+    <col min="40" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="32.25" customHeight="1">
+    <row r="1" spans="1:38" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +1942,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="20.25" customHeight="1">
+    <row r="2" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>5032728</v>
       </c>
@@ -2012,7 +2025,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="3" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8">
         <v>4995738</v>
       </c>
@@ -2108,7 +2121,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="4" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>5011587</v>
       </c>
@@ -2161,10 +2174,7 @@
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
-      <c r="Z4" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z4" s="11"/>
       <c r="AA4" s="9">
         <v>45</v>
       </c>
@@ -2184,7 +2194,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="5" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8">
         <v>2221543</v>
       </c>
@@ -2276,7 +2286,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="6" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8">
         <v>5018682</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="7" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>5046073</v>
       </c>
@@ -2417,10 +2427,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z7" s="11"/>
       <c r="AA7" s="9">
         <v>60</v>
       </c>
@@ -2444,7 +2451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="8" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8">
         <v>5027392</v>
       </c>
@@ -2501,10 +2508,7 @@
         <v>5.3</v>
       </c>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z8" s="11"/>
       <c r="AA8" s="9">
         <v>55</v>
       </c>
@@ -2530,7 +2534,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="9" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8">
         <v>2164684</v>
       </c>
@@ -2591,10 +2595,7 @@
         <v>4.3</v>
       </c>
       <c r="Y9" s="12"/>
-      <c r="Z9" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z9" s="11"/>
       <c r="AA9" s="9">
         <v>20</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="10" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>5018306</v>
       </c>
@@ -2683,10 +2684,7 @@
         <v>5</v>
       </c>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z10" s="11"/>
       <c r="AA10" s="9">
         <v>40</v>
       </c>
@@ -2716,7 +2714,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="11" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8">
         <v>6667885</v>
       </c>
@@ -2763,10 +2761,7 @@
         <v>4.2</v>
       </c>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z11" s="11"/>
       <c r="AA11" s="9">
         <v>60</v>
       </c>
@@ -2786,7 +2781,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="12" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
         <v>6709057</v>
       </c>
@@ -2841,10 +2836,7 @@
         <v>4.3</v>
       </c>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z12" s="11"/>
       <c r="AA12" s="9">
         <v>65</v>
       </c>
@@ -2866,7 +2858,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="13" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>2746173</v>
       </c>
@@ -2915,10 +2907,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z13" s="11"/>
       <c r="AA13" s="9">
         <v>60</v>
       </c>
@@ -2942,7 +2931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="14" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>5050122</v>
       </c>
@@ -2991,10 +2980,7 @@
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z14" s="11"/>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
@@ -3014,7 +3000,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="15" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>1577589</v>
       </c>
@@ -3061,10 +3047,7 @@
         <v>4.03</v>
       </c>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z15" s="11"/>
       <c r="AA15" s="9">
         <v>45</v>
       </c>
@@ -3092,7 +3075,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="16" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>4999011</v>
       </c>
@@ -3139,10 +3122,7 @@
         <v>5.13</v>
       </c>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z16" s="11"/>
       <c r="AA16" s="9">
         <v>55</v>
       </c>
@@ -3172,7 +3152,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="17" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
         <v>1925813</v>
       </c>
@@ -3229,10 +3209,7 @@
         <v>3</v>
       </c>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z17" s="11"/>
       <c r="AA17" s="9">
         <v>60</v>
       </c>
@@ -3256,7 +3233,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="18" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
         <v>4533890</v>
       </c>
@@ -3305,10 +3282,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="Y18" s="12"/>
-      <c r="Z18" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z18" s="11"/>
       <c r="AA18" s="9">
         <v>55</v>
       </c>
@@ -3334,7 +3308,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="19" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>4787158</v>
       </c>
@@ -3381,10 +3355,7 @@
         <v>4.28</v>
       </c>
       <c r="Y19" s="12"/>
-      <c r="Z19" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Z19" s="11"/>
       <c r="AA19" s="9">
         <v>45</v>
       </c>
@@ -3410,7 +3381,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="20" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>1835266</v>
       </c>
@@ -3491,7 +3462,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="21" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>2258916</v>
       </c>
@@ -3576,7 +3547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="22" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>1756911</v>
       </c>
@@ -3661,7 +3632,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="23" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
         <v>1814173</v>
       </c>
@@ -3744,7 +3715,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="24" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8">
         <v>2260316</v>
       </c>
@@ -3833,7 +3804,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="25" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8">
         <v>5987474</v>
       </c>
@@ -3920,7 +3891,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="26" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8">
         <v>2086841</v>
       </c>
@@ -4001,7 +3972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="27" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8">
         <v>5258594</v>
       </c>
@@ -4084,7 +4055,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="28" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8">
         <v>2395509</v>
       </c>
@@ -4173,7 +4144,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="29" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8">
         <v>5993118</v>
       </c>
@@ -4268,7 +4239,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="30" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8">
         <v>3760238</v>
       </c>
@@ -4353,7 +4324,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="31" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8">
         <v>1832860</v>
       </c>
@@ -4436,7 +4407,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8">
         <v>4747284</v>
       </c>
@@ -4523,7 +4494,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="33" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8">
         <v>2287369</v>
       </c>
@@ -4608,7 +4579,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="34" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="8">
         <v>2504298</v>
       </c>
@@ -4691,7 +4662,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="35" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13">
         <v>0.30496193999999999</v>
       </c>
@@ -4780,7 +4751,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="36" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8">
         <v>200277110</v>
       </c>
@@ -4877,7 +4848,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="37" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8">
         <v>0.80987655999999997</v>
       </c>
@@ -4968,7 +4939,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="38" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>0.80334351000000004</v>
       </c>
@@ -5063,7 +5034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="39" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8">
         <v>0.77030069999999995</v>
       </c>
@@ -5152,7 +5123,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="40" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8">
         <v>0.80696361999999999</v>
       </c>
@@ -5245,7 +5216,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="41" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8">
         <v>0.76941822000000004</v>
       </c>
@@ -5332,7 +5303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="42" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8">
         <v>0.80701712000000003</v>
       </c>
@@ -5425,7 +5396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="43" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="8">
         <v>0.80585675000000001</v>
       </c>
@@ -5508,7 +5479,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="44" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="8">
         <v>0.81069906999999997</v>
       </c>
@@ -5597,7 +5568,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="45" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="8">
         <v>0.72285809999999995</v>
       </c>
@@ -5693,7 +5664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="46" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="8">
         <v>0.80073901999999997</v>
       </c>
@@ -5784,7 +5755,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="47" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="8">
         <v>0.31742414000000002</v>
       </c>
@@ -5887,7 +5858,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="48" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8">
         <v>200199449</v>
       </c>
@@ -5974,7 +5945,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="49" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8">
         <v>200194183</v>
       </c>
@@ -6063,7 +6034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="50" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="8">
         <v>0.80433538999999998</v>
       </c>
@@ -6156,7 +6127,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="51" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="8">
         <v>0.75108019000000004</v>
       </c>
@@ -6243,7 +6214,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="52" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8">
         <v>0.75512228000000003</v>
       </c>
@@ -6340,7 +6311,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="53" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="8">
         <v>0.81431001999999997</v>
       </c>
@@ -6419,7 +6390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="54" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18"/>
       <c r="B54" s="12"/>
       <c r="C54" s="10"/>
@@ -6459,7 +6430,7 @@
       <c r="AK54" s="10"/>
       <c r="AL54" s="12"/>
     </row>
-    <row r="55" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="55" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="18"/>
       <c r="B55" s="12"/>
       <c r="C55" s="10"/>
@@ -6499,7 +6470,7 @@
       <c r="AK55" s="10"/>
       <c r="AL55" s="12"/>
     </row>
-    <row r="56" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="56" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="18"/>
       <c r="B56" s="12"/>
       <c r="C56" s="10"/>
@@ -6539,7 +6510,7 @@
       <c r="AK56" s="10"/>
       <c r="AL56" s="12"/>
     </row>
-    <row r="57" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="57" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="18"/>
       <c r="B57" s="12"/>
       <c r="C57" s="10"/>
@@ -6579,7 +6550,7 @@
       <c r="AK57" s="10"/>
       <c r="AL57" s="12"/>
     </row>
-    <row r="58" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="58" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="18"/>
       <c r="B58" s="12"/>
       <c r="C58" s="10"/>
@@ -6619,7 +6590,7 @@
       <c r="AK58" s="10"/>
       <c r="AL58" s="12"/>
     </row>
-    <row r="59" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="59" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="18"/>
       <c r="B59" s="12"/>
       <c r="C59" s="10"/>
@@ -6659,7 +6630,7 @@
       <c r="AK59" s="10"/>
       <c r="AL59" s="12"/>
     </row>
-    <row r="60" spans="1:38" ht="20.149999999999999" customHeight="1">
+    <row r="60" spans="1:38" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="18"/>
       <c r="B60" s="12"/>
       <c r="C60" s="10"/>

</xml_diff>